<commit_message>
Filled out Time Estimate sheet
</commit_message>
<xml_diff>
--- a/02 - EstimatingWorkSheet_Tyler.xlsx
+++ b/02 - EstimatingWorkSheet_Tyler.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\COMP_253_SystemsProject\SweetShop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\SweetShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
   <si>
     <t>Duration Estimating Worksheet</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>SweetSpot</t>
+  </si>
+  <si>
+    <t>Database</t>
   </si>
 </sst>
 </file>
@@ -539,6 +542,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -562,12 +571,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -865,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,31 +880,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
+      <c r="B2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
@@ -932,16 +935,16 @@
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:15" ht="86.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="24" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -959,18 +962,18 @@
       <c r="J7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="24" t="s">
+      <c r="K7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="6" t="s">
         <v>6</v>
       </c>
@@ -978,546 +981,672 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="11"/>
-      <c r="K8" s="26" t="s">
+      <c r="K8" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="27"/>
-      <c r="M8" s="28" t="s">
+      <c r="L8" s="29"/>
+      <c r="M8" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="28"/>
+      <c r="N8" s="30"/>
     </row>
     <row r="9" spans="1:15" ht="28.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="C9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
       <c r="F9" s="8">
         <f>(C9+4*D9+E9)/6</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
       </c>
       <c r="H9" s="8">
         <f>$F9+$G9</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I9" s="9">
         <f>H9/2</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="12"/>
+        <v>0.625</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K9" s="8"/>
       <c r="L9" s="17">
         <f>K9*H9</f>
         <v>0</v>
       </c>
       <c r="M9" s="13"/>
-      <c r="N9" s="17">
+      <c r="N9" s="17" t="e">
         <f>M9*J9</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="C10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>3</v>
+      </c>
       <c r="F10" s="8">
         <f>(C10+4*D10+E10)/6</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G10" s="3">
         <v>0</v>
       </c>
       <c r="H10" s="8">
         <f t="shared" ref="H10:H14" si="0">F10+G10</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I10" s="9">
         <f t="shared" ref="I10:I14" si="1">H10/2</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="12"/>
+        <v>0.625</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K10" s="12"/>
       <c r="L10" s="17">
         <f t="shared" ref="L10:L92" si="2">K10*H10</f>
         <v>0</v>
       </c>
       <c r="M10" s="13"/>
-      <c r="N10" s="17">
+      <c r="N10" s="17" t="e">
         <f t="shared" ref="N10:N73" si="3">M10*J10</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="C11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>3</v>
+      </c>
       <c r="F11" s="8">
         <f t="shared" ref="F11:F14" si="4">(C11+4*D11+E11)/6</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G11" s="3">
         <v>0</v>
       </c>
       <c r="H11" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I11" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="12"/>
+        <v>0.625</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K11" s="12"/>
       <c r="L11" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M11" s="13"/>
-      <c r="N11" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N11" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="C12" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>3</v>
+      </c>
       <c r="F12" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G12" s="3">
         <v>0</v>
       </c>
       <c r="H12" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I12" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="13"/>
+        <v>0.625</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K12" s="14"/>
       <c r="L12" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M12" s="13"/>
-      <c r="N12" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N12" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="C13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3</v>
+      </c>
       <c r="F13" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G13" s="3">
         <v>0</v>
       </c>
       <c r="H13" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I13" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="12"/>
+        <v>0.625</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K13" s="14"/>
       <c r="L13" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M13" s="13"/>
-      <c r="N13" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N13" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="C14" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>3</v>
+      </c>
       <c r="F14" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G14" s="3">
         <v>0</v>
       </c>
       <c r="H14" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I14" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="12"/>
+        <v>0.625</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K14" s="14"/>
       <c r="L14" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M14" s="13"/>
-      <c r="N14" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N14" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="C15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>3</v>
+      </c>
       <c r="F15" s="8">
         <f>(C15+4*D15+E15)/6</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G15" s="3">
         <v>0</v>
       </c>
       <c r="H15" s="8">
         <f t="shared" ref="H15:H24" si="5">F15+G15</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I15" s="9">
         <f t="shared" ref="I15:I24" si="6">H15/2</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="12"/>
+        <v>0.625</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K15" s="12"/>
       <c r="L15" s="17">
         <f t="shared" ref="L15:L24" si="7">K15*H15</f>
         <v>0</v>
       </c>
       <c r="M15" s="13"/>
-      <c r="N15" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N15" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="C16" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>3</v>
+      </c>
       <c r="F16" s="8">
         <f t="shared" ref="F16:F19" si="8">(C16+4*D16+E16)/6</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G16" s="3">
         <v>0</v>
       </c>
       <c r="H16" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I16" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="12"/>
+        <v>0.625</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K16" s="12"/>
       <c r="L16" s="17">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M16" s="13"/>
-      <c r="N16" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N16" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="C17" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <v>3</v>
+      </c>
       <c r="F17" s="8">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G17" s="3">
         <v>0</v>
       </c>
       <c r="H17" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I17" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="13"/>
+        <v>0.625</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K17" s="14"/>
       <c r="L17" s="17">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M17" s="13"/>
-      <c r="N17" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N17" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="C18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <v>3</v>
+      </c>
       <c r="F18" s="8">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G18" s="3">
         <v>0</v>
       </c>
       <c r="H18" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I18" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="12"/>
+        <v>0.625</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K18" s="14"/>
       <c r="L18" s="17">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M18" s="13"/>
-      <c r="N18" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N18" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="C19" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>3</v>
+      </c>
       <c r="F19" s="8">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G19" s="3">
         <v>0</v>
       </c>
       <c r="H19" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I19" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="12"/>
+        <v>0.625</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K19" s="14"/>
       <c r="L19" s="17">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M19" s="13"/>
-      <c r="N19" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N19" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="20" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="C20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>3</v>
+      </c>
       <c r="F20" s="8">
         <f>(C20+4*D20+E20)/6</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G20" s="3">
         <v>0</v>
       </c>
       <c r="H20" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I20" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="12"/>
+        <v>0.625</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K20" s="12"/>
       <c r="L20" s="17">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M20" s="13"/>
-      <c r="N20" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N20" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="21" spans="2:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="C21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <v>3</v>
+      </c>
       <c r="F21" s="8">
         <f t="shared" ref="F21:F24" si="9">(C21+4*D21+E21)/6</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G21" s="3">
         <v>0</v>
       </c>
       <c r="H21" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I21" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="12"/>
+        <v>0.625</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K21" s="12"/>
       <c r="L21" s="17">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M21" s="13"/>
-      <c r="N21" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N21" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="22" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="C22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>3</v>
+      </c>
       <c r="F22" s="8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G22" s="3">
         <v>0</v>
       </c>
       <c r="H22" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I22" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="13"/>
+        <v>0.625</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K22" s="14"/>
       <c r="L22" s="17">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M22" s="13"/>
-      <c r="N22" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N22" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="23" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="C23" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>3</v>
+      </c>
       <c r="F23" s="8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G23" s="3">
         <v>0</v>
       </c>
       <c r="H23" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I23" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="12"/>
+        <v>0.625</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K23" s="14"/>
       <c r="L23" s="17">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M23" s="13"/>
-      <c r="N23" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N23" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="C24" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3">
+        <v>3</v>
+      </c>
       <c r="F24" s="8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G24" s="3">
         <v>0</v>
       </c>
       <c r="H24" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I24" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="J24" s="12"/>
       <c r="K24" s="14"/>
@@ -1532,26 +1661,32 @@
       </c>
     </row>
     <row r="25" spans="2:14" ht="53.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="C25" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="E25" s="3">
+        <v>3</v>
+      </c>
       <c r="F25" s="8">
         <f>(C25+4*D25+E25)/6</f>
-        <v>0</v>
+        <v>1.5833333333333333</v>
       </c>
       <c r="G25" s="3">
         <v>0</v>
       </c>
       <c r="H25" s="8">
         <f t="shared" ref="H25:H44" si="10">F25+G25</f>
-        <v>0</v>
+        <v>1.5833333333333333</v>
       </c>
       <c r="I25" s="9">
         <f t="shared" ref="I25:I44" si="11">H25/2</f>
-        <v>0</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
@@ -1566,26 +1701,32 @@
       </c>
     </row>
     <row r="26" spans="2:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="C26" s="3">
+        <v>3</v>
+      </c>
+      <c r="D26" s="3">
+        <v>6</v>
+      </c>
+      <c r="E26" s="3">
+        <v>9</v>
+      </c>
       <c r="F26" s="8">
         <f t="shared" ref="F26:F29" si="13">(C26+4*D26+E26)/6</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G26" s="3">
         <v>0</v>
       </c>
       <c r="H26" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I26" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
@@ -1600,26 +1741,32 @@
       </c>
     </row>
     <row r="27" spans="2:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
+      <c r="C27" s="4">
+        <v>1</v>
+      </c>
+      <c r="D27" s="4">
+        <v>3</v>
+      </c>
+      <c r="E27" s="4">
+        <v>5</v>
+      </c>
       <c r="F27" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G27" s="3">
         <v>0</v>
       </c>
       <c r="H27" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I27" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J27" s="13"/>
       <c r="K27" s="14"/>
@@ -1634,26 +1781,32 @@
       </c>
     </row>
     <row r="28" spans="2:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="C28" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E28" s="4">
+        <v>4</v>
+      </c>
       <c r="F28" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="G28" s="3">
         <v>0</v>
       </c>
       <c r="H28" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="I28" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.875</v>
       </c>
       <c r="J28" s="12"/>
       <c r="K28" s="14"/>
@@ -1668,26 +1821,32 @@
       </c>
     </row>
     <row r="29" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="C29" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E29" s="4">
+        <v>1.5</v>
+      </c>
       <c r="F29" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.46666666666666662</v>
       </c>
       <c r="G29" s="3">
         <v>0</v>
       </c>
       <c r="H29" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.46666666666666662</v>
       </c>
       <c r="I29" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.23333333333333331</v>
       </c>
       <c r="J29" s="12"/>
       <c r="K29" s="14"/>
@@ -1702,26 +1861,32 @@
       </c>
     </row>
     <row r="30" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
+        <v>2</v>
+      </c>
+      <c r="E30" s="3">
+        <v>6</v>
+      </c>
       <c r="F30" s="8">
         <f>(C30+4*D30+E30)/6</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="G30" s="3">
         <v>0</v>
       </c>
       <c r="H30" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="I30" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
@@ -1736,26 +1901,32 @@
       </c>
     </row>
     <row r="31" spans="2:14" ht="40.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="C31" s="3">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3">
+        <v>2</v>
+      </c>
+      <c r="E31" s="3">
+        <v>6</v>
+      </c>
       <c r="F31" s="8">
         <f t="shared" ref="F31:F34" si="14">(C31+4*D31+E31)/6</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="G31" s="3">
         <v>0</v>
       </c>
       <c r="H31" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="I31" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
@@ -1770,196 +1941,242 @@
       </c>
     </row>
     <row r="32" spans="2:14" ht="53.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="C32" s="3">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3">
+        <v>6</v>
+      </c>
       <c r="F32" s="8">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="G32" s="3">
         <v>0</v>
       </c>
       <c r="H32" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="I32" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J32" s="13"/>
+        <v>1.25</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K32" s="14"/>
       <c r="L32" s="17">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M32" s="13"/>
-      <c r="N32" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N32" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="33" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="C33" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3">
+        <v>3</v>
+      </c>
       <c r="F33" s="8">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="G33" s="3">
         <v>0</v>
       </c>
       <c r="H33" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I33" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="12"/>
+        <v>0.625</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K33" s="14"/>
       <c r="L33" s="17">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M33" s="13"/>
-      <c r="N33" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N33" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="34" spans="2:14" ht="40.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="C34" s="4">
+        <v>1</v>
+      </c>
+      <c r="D34" s="4">
+        <v>2</v>
+      </c>
+      <c r="E34" s="4">
+        <v>4</v>
+      </c>
       <c r="F34" s="8">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2.1666666666666665</v>
       </c>
       <c r="G34" s="3">
         <v>0</v>
       </c>
       <c r="H34" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2.1666666666666665</v>
       </c>
       <c r="I34" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J34" s="12"/>
+        <v>1.0833333333333333</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K34" s="14"/>
       <c r="L34" s="17">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M34" s="13"/>
-      <c r="N34" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N34" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="35" spans="2:14" ht="40.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="C35" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3">
+        <v>1.5</v>
+      </c>
       <c r="F35" s="8">
         <f>(C35+4*D35+E35)/6</f>
-        <v>0</v>
+        <v>0.95000000000000007</v>
       </c>
       <c r="G35" s="3">
         <v>0</v>
       </c>
       <c r="H35" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.95000000000000007</v>
       </c>
       <c r="I35" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J35" s="12"/>
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K35" s="12"/>
       <c r="L35" s="17">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M35" s="13"/>
-      <c r="N35" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N35" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="36" spans="2:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="C36" s="3">
+        <v>1</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="E36" s="3">
+        <v>3</v>
+      </c>
       <c r="F36" s="8">
         <f t="shared" ref="F36:F39" si="15">(C36+4*D36+E36)/6</f>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="G36" s="3">
         <v>0</v>
       </c>
       <c r="H36" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="I36" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J36" s="12"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="K36" s="12"/>
       <c r="L36" s="17">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M36" s="13"/>
-      <c r="N36" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="N36" s="17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="37" spans="2:14" ht="40.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+      <c r="C37" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E37" s="4">
+        <v>2</v>
+      </c>
       <c r="F37" s="8">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="G37" s="3">
         <v>0</v>
       </c>
       <c r="H37" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="I37" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="J37" s="13"/>
       <c r="K37" s="14"/>
@@ -1974,26 +2191,32 @@
       </c>
     </row>
     <row r="38" spans="2:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
+      <c r="C38" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E38" s="4">
+        <v>1</v>
+      </c>
       <c r="F38" s="8">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.51666666666666672</v>
       </c>
       <c r="G38" s="3">
         <v>0</v>
       </c>
       <c r="H38" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.51666666666666672</v>
       </c>
       <c r="I38" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.25833333333333336</v>
       </c>
       <c r="J38" s="12"/>
       <c r="K38" s="14"/>
@@ -2008,26 +2231,32 @@
       </c>
     </row>
     <row r="39" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
+      <c r="C39" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1</v>
+      </c>
+      <c r="E39" s="4">
+        <v>1.5</v>
+      </c>
       <c r="F39" s="8">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.96666666666666667</v>
       </c>
       <c r="G39" s="3">
         <v>0</v>
       </c>
       <c r="H39" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.96666666666666667</v>
       </c>
       <c r="I39" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.48333333333333334</v>
       </c>
       <c r="J39" s="12"/>
       <c r="K39" s="14"/>
@@ -2042,26 +2271,32 @@
       </c>
     </row>
     <row r="40" spans="2:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="C40" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E40" s="3">
+        <v>1</v>
+      </c>
       <c r="F40" s="8">
         <f>(C40+4*D40+E40)/6</f>
-        <v>0</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="G40" s="3">
         <v>0</v>
       </c>
       <c r="H40" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="I40" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
@@ -2076,26 +2311,32 @@
       </c>
     </row>
     <row r="41" spans="2:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="29" t="s">
+      <c r="B41" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="C41" s="3">
+        <v>2</v>
+      </c>
+      <c r="D41" s="3">
+        <v>3</v>
+      </c>
+      <c r="E41" s="3">
+        <v>5</v>
+      </c>
       <c r="F41" s="8">
         <f t="shared" ref="F41:F44" si="16">(C41+4*D41+E41)/6</f>
-        <v>0</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="G41" s="3">
         <v>0</v>
       </c>
       <c r="H41" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="I41" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.5833333333333333</v>
       </c>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
@@ -2110,26 +2351,32 @@
       </c>
     </row>
     <row r="42" spans="2:14" ht="40.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
+      <c r="D42" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E42" s="4">
+        <v>4</v>
+      </c>
       <c r="F42" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="G42" s="3">
         <v>0</v>
       </c>
       <c r="H42" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="I42" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="J42" s="13"/>
       <c r="K42" s="14"/>
@@ -2144,26 +2391,32 @@
       </c>
     </row>
     <row r="43" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
+      <c r="C43" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1</v>
+      </c>
+      <c r="E43" s="4">
+        <v>2.5</v>
+      </c>
       <c r="F43" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="G43" s="3">
         <v>0</v>
       </c>
       <c r="H43" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="I43" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="J43" s="12"/>
       <c r="K43" s="14"/>
@@ -2178,26 +2431,32 @@
       </c>
     </row>
     <row r="44" spans="2:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
+      <c r="C44" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1</v>
+      </c>
+      <c r="E44" s="4">
+        <v>2.5</v>
+      </c>
       <c r="F44" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="G44" s="3">
         <v>0</v>
       </c>
       <c r="H44" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="I44" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="J44" s="12"/>
       <c r="K44" s="14"/>
@@ -2212,26 +2471,32 @@
       </c>
     </row>
     <row r="45" spans="2:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="29" t="s">
+      <c r="B45" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
+      <c r="C45" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D45" s="4">
+        <v>1</v>
+      </c>
+      <c r="E45" s="4">
+        <v>2.5</v>
+      </c>
       <c r="F45" s="8">
         <f>(C45+4*D45+E45)/6</f>
-        <v>0</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="G45" s="3">
         <v>0</v>
       </c>
       <c r="H45" s="8">
         <f t="shared" ref="H45:H84" si="17">F45+G45</f>
-        <v>0</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="I45" s="9">
         <f t="shared" ref="I45:I84" si="18">H45/2</f>
-        <v>0</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
@@ -2246,26 +2511,32 @@
       </c>
     </row>
     <row r="46" spans="2:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
+      <c r="C46" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
       <c r="F46" s="8">
         <f t="shared" ref="F46:F49" si="20">(C46+4*D46+E46)/6</f>
-        <v>0</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="G46" s="3">
         <v>0</v>
       </c>
       <c r="H46" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="I46" s="9">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
@@ -2280,26 +2551,32 @@
       </c>
     </row>
     <row r="47" spans="2:14" ht="53.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
+      <c r="C47" s="4">
+        <v>1</v>
+      </c>
+      <c r="D47" s="4">
+        <v>2</v>
+      </c>
+      <c r="E47" s="4">
+        <v>3</v>
+      </c>
       <c r="F47" s="8">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G47" s="3">
         <v>0</v>
       </c>
       <c r="H47" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I47" s="9">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" s="13"/>
       <c r="K47" s="14"/>
@@ -2314,26 +2591,32 @@
       </c>
     </row>
     <row r="48" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="30" t="s">
+      <c r="B48" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
+      <c r="C48" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E48" s="4">
+        <v>1</v>
+      </c>
       <c r="F48" s="8">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="G48" s="3">
         <v>0</v>
       </c>
       <c r="H48" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="I48" s="9">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="J48" s="12"/>
       <c r="K48" s="14"/>
@@ -2348,26 +2631,32 @@
       </c>
     </row>
     <row r="49" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="30" t="s">
+      <c r="B49" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
+      <c r="C49" s="4">
+        <v>1</v>
+      </c>
+      <c r="D49" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E49" s="4">
+        <v>2.5</v>
+      </c>
       <c r="F49" s="8">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1.5833333333333333</v>
       </c>
       <c r="G49" s="3">
         <v>0</v>
       </c>
       <c r="H49" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1.5833333333333333</v>
       </c>
       <c r="I49" s="9">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="J49" s="12"/>
       <c r="K49" s="14"/>
@@ -2382,26 +2671,32 @@
       </c>
     </row>
     <row r="50" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="29" t="s">
+      <c r="B50" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
+      <c r="C50" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E50" s="4">
+        <v>1</v>
+      </c>
       <c r="F50" s="8">
         <f>(C50+4*D50+E50)/6</f>
-        <v>0</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="G50" s="3">
         <v>0</v>
       </c>
       <c r="H50" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="I50" s="9">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
@@ -2416,26 +2711,32 @@
       </c>
     </row>
     <row r="51" spans="2:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="29" t="s">
+      <c r="B51" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
+      <c r="C51" s="3">
+        <v>3</v>
+      </c>
+      <c r="D51" s="3">
+        <v>4</v>
+      </c>
+      <c r="E51" s="3">
+        <v>6</v>
+      </c>
       <c r="F51" s="8">
         <f t="shared" ref="F51:F54" si="21">(C51+4*D51+E51)/6</f>
-        <v>0</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="G51" s="3">
         <v>0</v>
       </c>
       <c r="H51" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="I51" s="9">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>2.0833333333333335</v>
       </c>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
@@ -2450,26 +2751,32 @@
       </c>
     </row>
     <row r="52" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="30" t="s">
+      <c r="B52" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
+      <c r="C52" s="4">
+        <v>1</v>
+      </c>
+      <c r="D52" s="4">
+        <v>2</v>
+      </c>
+      <c r="E52" s="4">
+        <v>3</v>
+      </c>
       <c r="F52" s="8">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G52" s="3">
         <v>0</v>
       </c>
       <c r="H52" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I52" s="9">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" s="13"/>
       <c r="K52" s="14"/>
@@ -2484,24 +2791,30 @@
       </c>
     </row>
     <row r="53" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="30"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="4">
+        <v>1</v>
+      </c>
+      <c r="D53" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E53" s="4">
+        <v>2</v>
+      </c>
       <c r="F53" s="8">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G53" s="3">
         <v>0</v>
       </c>
       <c r="H53" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I53" s="9">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J53" s="12"/>
       <c r="K53" s="14"/>
@@ -2516,24 +2829,30 @@
       </c>
     </row>
     <row r="54" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="30"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="4">
+        <v>1</v>
+      </c>
+      <c r="D54" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E54" s="4">
+        <v>2</v>
+      </c>
       <c r="F54" s="8">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G54" s="3">
         <v>0</v>
       </c>
       <c r="H54" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I54" s="9">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J54" s="12"/>
       <c r="K54" s="14"/>
@@ -2548,24 +2867,30 @@
       </c>
     </row>
     <row r="55" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="29"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="4">
+        <v>1</v>
+      </c>
+      <c r="D55" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E55" s="4">
+        <v>2</v>
+      </c>
       <c r="F55" s="8">
         <f>(C55+4*D55+E55)/6</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G55" s="3">
         <v>0</v>
       </c>
       <c r="H55" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I55" s="9">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J55" s="12"/>
       <c r="K55" s="12"/>
@@ -2580,24 +2905,30 @@
       </c>
     </row>
     <row r="56" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="29"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="4">
+        <v>1</v>
+      </c>
+      <c r="D56" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E56" s="4">
+        <v>2</v>
+      </c>
       <c r="F56" s="8">
         <f t="shared" ref="F56:F59" si="22">(C56+4*D56+E56)/6</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G56" s="3">
         <v>0</v>
       </c>
       <c r="H56" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I56" s="9">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
@@ -2612,24 +2943,30 @@
       </c>
     </row>
     <row r="57" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="30"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
+      <c r="B57" s="22"/>
+      <c r="C57" s="4">
+        <v>2</v>
+      </c>
+      <c r="D57" s="4">
+        <v>3</v>
+      </c>
+      <c r="E57" s="4">
+        <v>6</v>
+      </c>
       <c r="F57" s="8">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="G57" s="3">
         <v>0</v>
       </c>
       <c r="H57" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="I57" s="9">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="J57" s="13"/>
       <c r="K57" s="14"/>
@@ -2644,24 +2981,30 @@
       </c>
     </row>
     <row r="58" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="30"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="4">
+        <v>2</v>
+      </c>
+      <c r="D58" s="4">
+        <v>3</v>
+      </c>
+      <c r="E58" s="4">
+        <v>6</v>
+      </c>
       <c r="F58" s="8">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="G58" s="3">
         <v>0</v>
       </c>
       <c r="H58" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="I58" s="9">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="J58" s="12"/>
       <c r="K58" s="14"/>
@@ -2676,24 +3019,30 @@
       </c>
     </row>
     <row r="59" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="30"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="4">
+        <v>2</v>
+      </c>
+      <c r="D59" s="4">
+        <v>3</v>
+      </c>
+      <c r="E59" s="4">
+        <v>6</v>
+      </c>
       <c r="F59" s="8">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="G59" s="3">
         <v>0</v>
       </c>
       <c r="H59" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="I59" s="9">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="J59" s="12"/>
       <c r="K59" s="14"/>
@@ -2708,10 +3057,10 @@
       </c>
     </row>
     <row r="60" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="29"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
       <c r="F60" s="8">
         <f>(C60+4*D60+E60)/6</f>
         <v>0</v>
@@ -2740,7 +3089,7 @@
       </c>
     </row>
     <row r="61" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="29"/>
+      <c r="B61" s="21"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -2772,7 +3121,7 @@
       </c>
     </row>
     <row r="62" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="30"/>
+      <c r="B62" s="22"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -2804,7 +3153,7 @@
       </c>
     </row>
     <row r="63" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="30"/>
+      <c r="B63" s="22"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -2836,7 +3185,7 @@
       </c>
     </row>
     <row r="64" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="30"/>
+      <c r="B64" s="22"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
@@ -2868,7 +3217,7 @@
       </c>
     </row>
     <row r="65" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="29"/>
+      <c r="B65" s="21"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -2900,7 +3249,7 @@
       </c>
     </row>
     <row r="66" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="29"/>
+      <c r="B66" s="21"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -2932,7 +3281,7 @@
       </c>
     </row>
     <row r="67" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="30"/>
+      <c r="B67" s="22"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -2964,7 +3313,7 @@
       </c>
     </row>
     <row r="68" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="30"/>
+      <c r="B68" s="22"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -2996,7 +3345,7 @@
       </c>
     </row>
     <row r="69" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="30"/>
+      <c r="B69" s="22"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -3028,7 +3377,7 @@
       </c>
     </row>
     <row r="70" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="29"/>
+      <c r="B70" s="21"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
@@ -3060,7 +3409,7 @@
       </c>
     </row>
     <row r="71" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="29"/>
+      <c r="B71" s="21"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
@@ -3092,7 +3441,7 @@
       </c>
     </row>
     <row r="72" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="30"/>
+      <c r="B72" s="22"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -3124,7 +3473,7 @@
       </c>
     </row>
     <row r="73" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="30"/>
+      <c r="B73" s="22"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -3156,7 +3505,7 @@
       </c>
     </row>
     <row r="74" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="30"/>
+      <c r="B74" s="22"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -3188,7 +3537,7 @@
       </c>
     </row>
     <row r="75" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="29"/>
+      <c r="B75" s="21"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
@@ -3220,7 +3569,7 @@
       </c>
     </row>
     <row r="76" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="29"/>
+      <c r="B76" s="21"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
@@ -3252,7 +3601,7 @@
       </c>
     </row>
     <row r="77" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="30"/>
+      <c r="B77" s="22"/>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -3284,7 +3633,7 @@
       </c>
     </row>
     <row r="78" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="30"/>
+      <c r="B78" s="22"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
@@ -3316,7 +3665,7 @@
       </c>
     </row>
     <row r="79" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B79" s="30"/>
+      <c r="B79" s="22"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -3348,7 +3697,7 @@
       </c>
     </row>
     <row r="80" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B80" s="29"/>
+      <c r="B80" s="21"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
@@ -3380,7 +3729,7 @@
       </c>
     </row>
     <row r="81" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B81" s="29"/>
+      <c r="B81" s="21"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
@@ -3412,7 +3761,7 @@
       </c>
     </row>
     <row r="82" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B82" s="30"/>
+      <c r="B82" s="22"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
@@ -3444,7 +3793,7 @@
       </c>
     </row>
     <row r="83" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="30"/>
+      <c r="B83" s="22"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
@@ -3476,7 +3825,7 @@
       </c>
     </row>
     <row r="84" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B84" s="30"/>
+      <c r="B84" s="22"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
@@ -3508,7 +3857,7 @@
       </c>
     </row>
     <row r="85" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="29"/>
+      <c r="B85" s="21"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
@@ -3540,7 +3889,7 @@
       </c>
     </row>
     <row r="86" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="29"/>
+      <c r="B86" s="21"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
@@ -3572,7 +3921,7 @@
       </c>
     </row>
     <row r="87" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B87" s="30"/>
+      <c r="B87" s="22"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -3604,7 +3953,7 @@
       </c>
     </row>
     <row r="88" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B88" s="30"/>
+      <c r="B88" s="22"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -3636,7 +3985,7 @@
       </c>
     </row>
     <row r="89" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="30"/>
+      <c r="B89" s="22"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -3668,7 +4017,7 @@
       </c>
     </row>
     <row r="90" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B90" s="30"/>
+      <c r="B90" s="22"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
@@ -3700,7 +4049,7 @@
       </c>
     </row>
     <row r="91" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B91" s="30"/>
+      <c r="B91" s="22"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
@@ -3751,11 +4100,11 @@
       </c>
       <c r="H93" s="5">
         <f>SUM(H9:H91)</f>
-        <v>0</v>
+        <v>85.566666666666634</v>
       </c>
       <c r="I93" s="10">
         <f>H93/2</f>
-        <v>0</v>
+        <v>42.783333333333317</v>
       </c>
       <c r="J93" s="13"/>
       <c r="K93" s="5">
@@ -3770,9 +4119,9 @@
         <f>SUM(M9:M91)</f>
         <v>0</v>
       </c>
-      <c r="N93" s="5">
+      <c r="N93" s="5" t="e">
         <f>SUM(N9:N91)</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="94" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -3791,16 +4140,16 @@
       </c>
       <c r="H95" s="5">
         <f>H94-H93</f>
-        <v>0</v>
+        <v>-85.566666666666634</v>
       </c>
       <c r="I95" s="5"/>
       <c r="L95" s="20">
         <f>SUM(L10:L92)</f>
         <v>0</v>
       </c>
-      <c r="N95" s="20">
+      <c r="N95" s="20" t="e">
         <f>SUM(N10:N92)</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WBS EST almost done
</commit_message>
<xml_diff>
--- a/02 - EstimatingWorkSheet_Tyler.xlsx
+++ b/02 - EstimatingWorkSheet_Tyler.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\SweetShop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\COMP_253_SystemsProject\SweetShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -868,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>